<commit_message>
working code need ot combine sheets now
</commit_message>
<xml_diff>
--- a/LabSignup/LabSignup/bin/Debug/ExcelFiles/FacilitatorsSignInSheet.xlsx
+++ b/LabSignup/LabSignup/bin/Debug/ExcelFiles/FacilitatorsSignInSheet.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CODING\LabSignup\LabSignup\LabSignup\bin\Debug\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56CFBB4-0423-4995-A09C-56747788CFA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{751647F0-FDF9-4382-8775-068E267B392C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="420" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4065" yWindow="4365" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,131 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
-  <si>
-    <t>Facilitator Names</t>
-  </si>
-  <si>
-    <t>Facilitator Titles</t>
-  </si>
-  <si>
-    <t>Course Name</t>
-  </si>
-  <si>
-    <t>CNP</t>
-  </si>
-  <si>
-    <t>CNS</t>
-  </si>
-  <si>
-    <t>CRNA</t>
-  </si>
-  <si>
-    <t>DENTAL</t>
-  </si>
-  <si>
-    <t>EMS</t>
-  </si>
-  <si>
-    <t>FELLOW</t>
-  </si>
-  <si>
-    <t>HEALTH AIDE</t>
-  </si>
-  <si>
-    <t>ICT</t>
-  </si>
-  <si>
-    <t>LPN</t>
-  </si>
-  <si>
-    <t>MD</t>
-  </si>
-  <si>
-    <t>MED INTERN</t>
-  </si>
-  <si>
-    <t>MIT</t>
-  </si>
-  <si>
-    <t>NA/HT/MA/MSA</t>
-  </si>
-  <si>
-    <t>OCC THERAPY</t>
-  </si>
-  <si>
-    <t>OTHER</t>
-  </si>
-  <si>
-    <t>PCT</t>
-  </si>
-  <si>
-    <t>PHARM</t>
-  </si>
-  <si>
-    <t>PHY ASST</t>
-  </si>
-  <si>
-    <t>PHY THERAPY</t>
-  </si>
-  <si>
-    <t>POLICE</t>
-  </si>
-  <si>
-    <t>PSYCH</t>
-  </si>
-  <si>
-    <t>RADIOLOGY</t>
-  </si>
-  <si>
-    <t>REG DIETICIAN</t>
-  </si>
-  <si>
-    <t>RESIDENT</t>
-  </si>
-  <si>
-    <t>RN</t>
-  </si>
-  <si>
-    <t>RT</t>
-  </si>
-  <si>
-    <t>SNT</t>
-  </si>
-  <si>
-    <t>SOCIAL WORKER</t>
-  </si>
-  <si>
-    <t>STNA</t>
-  </si>
-  <si>
-    <t>STUDENT NURSE</t>
-  </si>
-  <si>
-    <t>SURGERY</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>test1</t>
-  </si>
-  <si>
-    <t>UPL</t>
-  </si>
-  <si>
-    <t>Total Facilitators</t>
-  </si>
-  <si>
-    <t>Total Facilitators Hours</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -460,140 +341,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM1"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="A1:XFD1"/>
+      <selection activeCell="G12" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" bestFit="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" bestFit="1" width="26.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG1" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH1" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="AI1" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="AJ1" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="AK1" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL1" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="AM1" s="0" t="s">
-        <v>38</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
LAST FIXES for not updating attednee lists
</commit_message>
<xml_diff>
--- a/LabSignup/LabSignup/bin/Debug/ExcelFiles/FacilitatorsSignInSheet.xlsx
+++ b/LabSignup/LabSignup/bin/Debug/ExcelFiles/FacilitatorsSignInSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CODING\LabSignup\LabSignup\LabSignup\bin\Debug\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B9471F1-5882-4FC3-A0B6-F4C2288B20BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46F5BC0-DC04-460A-8770-387D8D42228C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29655" yWindow="2160" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1935" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -344,7 +344,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="A1:XFD1048576"/>
+      <selection activeCell="N12" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>